<commit_message>
feat: update GHCP Daily Capture Scorecard Template
</commit_message>
<xml_diff>
--- a/metrics/GHCP_Daily_Capture_Scorecard_Template.xlsx
+++ b/metrics/GHCP_Daily_Capture_Scorecard_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://avanade-my.sharepoint.com/personal/marcel_lupo_avanade_com/Documents/Avanade/Projects/NBS/Generalised/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcel.lupo\Downloads\OneDrive_1_26-01-2026\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_8FC8D49209A02FBA369011EB02AFB51ECB53CBBB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D02F583-6A2B-4F9C-8AA7-D649E87D891B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBED34C5-FBAB-40BB-894E-01084C67722E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -21,15 +21,18 @@
     <sheet name="Lists" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="Confidence">Lists!$B5:$D5</definedName>
-    <definedName name="Helpfulness1to5">Lists!$B7:$F7</definedName>
-    <definedName name="PainPoints">Lists!$B11:$L11</definedName>
-    <definedName name="Rework">Lists!$B9:$D9</definedName>
-    <definedName name="UseType">Lists!$B13:$I13</definedName>
-    <definedName name="YesNo">Lists!$B3:$C3</definedName>
+    <definedName name="Confidence">Lists!$B$5:$D$5</definedName>
+    <definedName name="Helpfulness1to5">Lists!$B$7:$F$7</definedName>
+    <definedName name="PainPoints">Lists!$B$11:$L$11</definedName>
+    <definedName name="Rework">Lists!$B$9:$D$9</definedName>
+    <definedName name="UseType">Lists!$B$13:$I$13</definedName>
+    <definedName name="YesNo">Lists!$B$3:$C$3</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -46,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="126">
   <si>
     <t>GitHub Copilot (GHCP) Daily Capture + Scorecard Template</t>
   </si>
@@ -376,21 +379,6 @@
     <t>Helpfulness1to5</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
     <t>Rework</t>
   </si>
   <si>
@@ -425,6 +413,33 @@
   </si>
   <si>
     <t>Learning/Exploration</t>
+  </si>
+  <si>
+    <t>Sprint1</t>
+  </si>
+  <si>
+    <t>Sprint2</t>
+  </si>
+  <si>
+    <t>TeamA</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Ash</t>
+  </si>
+  <si>
+    <t>Pete</t>
+  </si>
+  <si>
+    <t>Dev</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>Tester</t>
   </si>
 </sst>
 </file>
@@ -436,7 +451,7 @@
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -474,6 +489,19 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -521,7 +549,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -616,6 +644,22 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,9 +740,9 @@
           </c:spPr>
           <c:invertIfNegative val="1"/>
           <c:cat>
-            <c:multiLvlStrRef>
+            <c:strRef>
               <c:f>Dashboard!$A$9:$A$38</c:f>
-            </c:multiLvlStrRef>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -824,6 +868,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -915,9 +960,9 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:multiLvlStrRef>
+            <c:strRef>
               <c:f>Dashboard!$A$9:$A$38</c:f>
-            </c:multiLvlStrRef>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1044,6 +1089,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1134,9 +1180,9 @@
           </c:spPr>
           <c:invertIfNegative val="1"/>
           <c:cat>
-            <c:multiLvlStrRef>
+            <c:strRef>
               <c:f>Dashboard!$A$9:$A$38</c:f>
-            </c:multiLvlStrRef>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1262,6 +1308,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1650,7 +1697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -1714,13 +1761,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R201"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:XFD1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
@@ -1762,7 +1809,7 @@
       <c r="G1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="40" t="s">
         <v>16</v>
       </c>
       <c r="I1" s="4" t="s">
@@ -1797,103 +1844,273 @@
       </c>
     </row>
     <row r="2" spans="1:18" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="5"/>
+      <c r="A2" s="5">
+        <v>46029</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="I2" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="8">
+        <v>120</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="L2" s="43">
+        <v>2</v>
+      </c>
+      <c r="M2" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="O2" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="P2" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q2" s="41">
+        <v>46030</v>
+      </c>
       <c r="R2" s="6"/>
     </row>
     <row r="3" spans="1:18" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="5"/>
+      <c r="A3" s="5">
+        <v>46029</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="H3" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="I3" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="J3" s="8">
+        <v>-30</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="L3" s="43">
+        <v>1</v>
+      </c>
+      <c r="M3" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="O3" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="P3" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q3" s="41">
+        <v>46030</v>
+      </c>
       <c r="R3" s="6"/>
     </row>
     <row r="4" spans="1:18" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="5"/>
+      <c r="A4" s="5">
+        <v>46036</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="G4" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="H4" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="I4" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="J4" s="8">
+        <v>40</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="L4" s="43">
+        <v>4</v>
+      </c>
+      <c r="M4" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="O4" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="P4" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q4" s="41">
+        <v>46037</v>
+      </c>
       <c r="R4" s="6"/>
     </row>
     <row r="5" spans="1:18" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="5"/>
+      <c r="A5" s="5">
+        <v>46036</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="I5" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="J5" s="8">
+        <v>60</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="L5" s="43">
+        <v>4</v>
+      </c>
+      <c r="M5" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="O5" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="P5" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q5" s="41">
+        <v>46037</v>
+      </c>
       <c r="R5" s="6"/>
     </row>
     <row r="6" spans="1:18" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="5"/>
+      <c r="A6" s="5">
+        <v>46036</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="G6" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="H6" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="J6" s="8">
+        <v>60</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="L6" s="43">
+        <v>3</v>
+      </c>
+      <c r="M6" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="O6" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="P6" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q6" s="41">
+        <v>46037</v>
+      </c>
       <c r="R6" s="6"/>
     </row>
     <row r="7" spans="1:18" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -5797,6 +6014,26 @@
       <c r="R201" s="6"/>
     </row>
   </sheetData>
+  <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576 O1:O1048576" xr:uid="{26795AEE-6C0E-4813-AD97-1BF2A1474822}">
+      <formula1>YesNo</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:I1048576" xr:uid="{89A1EC40-8FBE-4D16-A1AA-0863ADC9D0CF}">
+      <formula1>UseType</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K1048576" xr:uid="{B18F6602-5F71-4422-9244-062C67E0089E}">
+      <formula1>Confidence</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1:L1048576" xr:uid="{5C22A4AE-9663-4A0F-A9EA-D5BA49A8155A}">
+      <formula1>Helpfulness1to5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1:N1048576" xr:uid="{09581579-8A0F-47B1-9199-8E6A41A0E223}">
+      <formula1>PainPoints</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M201" xr:uid="{80F10603-DF71-4C44-AD37-6C811F3E62EE}">
+      <formula1>Rework</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -5809,7 +6046,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A5" sqref="A1:XFD1048576"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5872,7 +6109,7 @@
       </c>
       <c r="C9" s="15">
         <f>COUNTIFS('Daily Capture'!$A$2:$A$201,"&gt;="&amp;$B$5,'Daily Capture'!$A$2:$A$201,"&lt;="&amp;$B$6,'Daily Capture'!$B$2:$B$201,IF($B$3="","*", $B$3),'Daily Capture'!$C$2:$C$201,IF($B$4="","*", $B$4),'Daily Capture'!$E$2:$E$201,"&lt;&gt;")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -5882,9 +6119,9 @@
       <c r="B10" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="16" t="str">
+      <c r="C10" s="16">
         <f>IF($C$9=0,"",COUNTIFS('Daily Capture'!$A$2:$A$201,"&gt;="&amp;$B$5,'Daily Capture'!$A$2:$A$201,"&lt;="&amp;$B$6,'Daily Capture'!$B$2:$B$201,IF($B$3="","*", $B$3),'Daily Capture'!$C$2:$C$201,IF($B$4="","*", $B$4),'Daily Capture'!$G$2:$G$201,"Yes")/$C$9)</f>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -5894,9 +6131,9 @@
       <c r="B11" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="15" t="str">
+      <c r="C11" s="15">
         <f>IF($C$9=0,"",SUMIFS('Daily Capture'!$J$2:$J$201,'Daily Capture'!$A$2:$A$201,"&gt;="&amp;$B$5,'Daily Capture'!$A$2:$A$201,"&lt;="&amp;$B$6,'Daily Capture'!$B$2:$B$201,IF($B$3="","*", $B$3),'Daily Capture'!$C$2:$C$201,IF($B$4="","*", $B$4)))</f>
-        <v/>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -5906,9 +6143,9 @@
       <c r="B12" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="17" t="str">
+      <c r="C12" s="17">
         <f>IF($C$11="","",$C$11/60)</f>
-        <v/>
+        <v>4.166666666666667</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -5918,9 +6155,9 @@
       <c r="B13" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="17" t="str">
+      <c r="C13" s="17">
         <f>IF($C$9=0,"",AVERAGEIFS('Daily Capture'!$L$2:$L$201,'Daily Capture'!$A$2:$A$201,"&gt;="&amp;$B$5,'Daily Capture'!$A$2:$A$201,"&lt;="&amp;$B$6,'Daily Capture'!$B$2:$B$201,IF($B$3="","*", $B$3),'Daily Capture'!$C$2:$C$201,IF($B$4="","*", $B$4),'Daily Capture'!$L$2:$L$201,"&gt;0"))</f>
-        <v/>
+        <v>2.8</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -5930,9 +6167,9 @@
       <c r="B14" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="16" t="str">
+      <c r="C14" s="16">
         <f>IF($C$9=0,"",(COUNTIFS('Daily Capture'!$A$2:$A$201,"&gt;="&amp;$B$5,'Daily Capture'!$A$2:$A$201,"&lt;="&amp;$B$6,'Daily Capture'!$B$2:$B$201,IF($B$3="","*", $B$3),'Daily Capture'!$C$2:$C$201,IF($B$4="","*", $B$4),'Daily Capture'!$M$2:$M$201,"Some")+COUNTIFS('Daily Capture'!$A$2:$A$201,"&gt;="&amp;$B$5,'Daily Capture'!$A$2:$A$201,"&lt;="&amp;$B$6,'Daily Capture'!$B$2:$B$201,IF($B$3="","*", $B$3),'Daily Capture'!$C$2:$C$201,IF($B$4="","*", $B$4),'Daily Capture'!$M$2:$M$201,"A lot"))/$C$9)</f>
-        <v/>
+        <v>0.6</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -5959,11 +6196,11 @@
       </c>
       <c r="B18" s="19">
         <f>COUNTIFS('Daily Capture'!$A$2:$A$201,"&gt;="&amp;$B$5,'Daily Capture'!$A$2:$A$201,"&lt;="&amp;$B$6,'Daily Capture'!$B$2:$B$201,IF($B$3="","*", $B$3),'Daily Capture'!$C$2:$C$201,IF($B$4="","*", $B$4),'Daily Capture'!$N$2:$N$201,$A18)</f>
-        <v>0</v>
-      </c>
-      <c r="C18" s="20" t="str">
+        <v>2</v>
+      </c>
+      <c r="C18" s="20">
         <f t="shared" ref="C18:C28" si="0">IF($C$9=0,"",$B18/$C$9)</f>
-        <v/>
+        <v>0.4</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -5972,11 +6209,11 @@
       </c>
       <c r="B19" s="19">
         <f>COUNTIFS('Daily Capture'!$A$2:$A$201,"&gt;="&amp;$B$5,'Daily Capture'!$A$2:$A$201,"&lt;="&amp;$B$6,'Daily Capture'!$B$2:$B$201,IF($B$3="","*", $B$3),'Daily Capture'!$C$2:$C$201,IF($B$4="","*", $B$4),'Daily Capture'!$N$2:$N$201,$A19)</f>
-        <v>0</v>
-      </c>
-      <c r="C19" s="20" t="str">
+        <v>1</v>
+      </c>
+      <c r="C19" s="20">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0.2</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -5987,9 +6224,9 @@
         <f>COUNTIFS('Daily Capture'!$A$2:$A$201,"&gt;="&amp;$B$5,'Daily Capture'!$A$2:$A$201,"&lt;="&amp;$B$6,'Daily Capture'!$B$2:$B$201,IF($B$3="","*", $B$3),'Daily Capture'!$C$2:$C$201,IF($B$4="","*", $B$4),'Daily Capture'!$N$2:$N$201,$A20)</f>
         <v>0</v>
       </c>
-      <c r="C20" s="20" t="str">
+      <c r="C20" s="20">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -5998,11 +6235,11 @@
       </c>
       <c r="B21" s="19">
         <f>COUNTIFS('Daily Capture'!$A$2:$A$201,"&gt;="&amp;$B$5,'Daily Capture'!$A$2:$A$201,"&lt;="&amp;$B$6,'Daily Capture'!$B$2:$B$201,IF($B$3="","*", $B$3),'Daily Capture'!$C$2:$C$201,IF($B$4="","*", $B$4),'Daily Capture'!$N$2:$N$201,$A21)</f>
-        <v>0</v>
-      </c>
-      <c r="C21" s="20" t="str">
+        <v>1</v>
+      </c>
+      <c r="C21" s="20">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0.2</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -6011,11 +6248,11 @@
       </c>
       <c r="B22" s="19">
         <f>COUNTIFS('Daily Capture'!$A$2:$A$201,"&gt;="&amp;$B$5,'Daily Capture'!$A$2:$A$201,"&lt;="&amp;$B$6,'Daily Capture'!$B$2:$B$201,IF($B$3="","*", $B$3),'Daily Capture'!$C$2:$C$201,IF($B$4="","*", $B$4),'Daily Capture'!$N$2:$N$201,$A22)</f>
-        <v>0</v>
-      </c>
-      <c r="C22" s="20" t="str">
+        <v>1</v>
+      </c>
+      <c r="C22" s="20">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0.2</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -6026,9 +6263,9 @@
         <f>COUNTIFS('Daily Capture'!$A$2:$A$201,"&gt;="&amp;$B$5,'Daily Capture'!$A$2:$A$201,"&lt;="&amp;$B$6,'Daily Capture'!$B$2:$B$201,IF($B$3="","*", $B$3),'Daily Capture'!$C$2:$C$201,IF($B$4="","*", $B$4),'Daily Capture'!$N$2:$N$201,$A23)</f>
         <v>0</v>
       </c>
-      <c r="C23" s="20" t="str">
+      <c r="C23" s="20">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -6039,9 +6276,9 @@
         <f>COUNTIFS('Daily Capture'!$A$2:$A$201,"&gt;="&amp;$B$5,'Daily Capture'!$A$2:$A$201,"&lt;="&amp;$B$6,'Daily Capture'!$B$2:$B$201,IF($B$3="","*", $B$3),'Daily Capture'!$C$2:$C$201,IF($B$4="","*", $B$4),'Daily Capture'!$N$2:$N$201,$A24)</f>
         <v>0</v>
       </c>
-      <c r="C24" s="20" t="str">
+      <c r="C24" s="20">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -6052,9 +6289,9 @@
         <f>COUNTIFS('Daily Capture'!$A$2:$A$201,"&gt;="&amp;$B$5,'Daily Capture'!$A$2:$A$201,"&lt;="&amp;$B$6,'Daily Capture'!$B$2:$B$201,IF($B$3="","*", $B$3),'Daily Capture'!$C$2:$C$201,IF($B$4="","*", $B$4),'Daily Capture'!$N$2:$N$201,$A25)</f>
         <v>0</v>
       </c>
-      <c r="C25" s="20" t="str">
+      <c r="C25" s="20">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -6065,9 +6302,9 @@
         <f>COUNTIFS('Daily Capture'!$A$2:$A$201,"&gt;="&amp;$B$5,'Daily Capture'!$A$2:$A$201,"&lt;="&amp;$B$6,'Daily Capture'!$B$2:$B$201,IF($B$3="","*", $B$3),'Daily Capture'!$C$2:$C$201,IF($B$4="","*", $B$4),'Daily Capture'!$N$2:$N$201,$A26)</f>
         <v>0</v>
       </c>
-      <c r="C26" s="20" t="str">
+      <c r="C26" s="20">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -6078,9 +6315,9 @@
         <f>COUNTIFS('Daily Capture'!$A$2:$A$201,"&gt;="&amp;$B$5,'Daily Capture'!$A$2:$A$201,"&lt;="&amp;$B$6,'Daily Capture'!$B$2:$B$201,IF($B$3="","*", $B$3),'Daily Capture'!$C$2:$C$201,IF($B$4="","*", $B$4),'Daily Capture'!$N$2:$N$201,$A27)</f>
         <v>0</v>
       </c>
-      <c r="C27" s="20" t="str">
+      <c r="C27" s="20">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -6091,9 +6328,9 @@
         <f>COUNTIFS('Daily Capture'!$A$2:$A$201,"&gt;="&amp;$B$5,'Daily Capture'!$A$2:$A$201,"&lt;="&amp;$B$6,'Daily Capture'!$B$2:$B$201,IF($B$3="","*", $B$3),'Daily Capture'!$C$2:$C$201,IF($B$4="","*", $B$4),'Daily Capture'!$N$2:$N$201,$A28)</f>
         <v>0</v>
       </c>
-      <c r="C28" s="20" t="str">
+      <c r="C28" s="20">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -6112,7 +6349,7 @@
       </c>
       <c r="B31" s="10" t="str">
         <f>IF($C$9=0,"",INDEX($A$18:$A$28, MATCH(MAX($B$18:$B$28), $B$18:$B$28, 0)))</f>
-        <v/>
+        <v>None</v>
       </c>
     </row>
   </sheetData>
@@ -6127,8 +6364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView showGridLines="0" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6152,7 +6389,7 @@
     <col min="17" max="19" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="93.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>62</v>
       </c>
@@ -8552,7 +8789,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8606,39 +8843,39 @@
       <c r="A7" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="B7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D7" t="s">
-        <v>107</v>
-      </c>
-      <c r="E7" t="s">
-        <v>108</v>
-      </c>
-      <c r="F7" t="s">
-        <v>109</v>
+      <c r="B7" s="42">
+        <v>1</v>
+      </c>
+      <c r="C7" s="42">
+        <v>2</v>
+      </c>
+      <c r="D7" s="42">
+        <v>3</v>
+      </c>
+      <c r="E7" s="42">
+        <v>4</v>
+      </c>
+      <c r="F7" s="42">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B9" t="s">
         <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D9" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B11" t="s">
         <v>50</v>
@@ -8676,28 +8913,28 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" t="s">
+        <v>112</v>
+      </c>
+      <c r="E13" t="s">
+        <v>113</v>
+      </c>
+      <c r="F13" t="s">
         <v>114</v>
       </c>
-      <c r="B13" t="s">
+      <c r="G13" t="s">
         <v>115</v>
       </c>
-      <c r="C13" t="s">
+      <c r="H13" t="s">
         <v>116</v>
-      </c>
-      <c r="D13" t="s">
-        <v>117</v>
-      </c>
-      <c r="E13" t="s">
-        <v>118</v>
-      </c>
-      <c r="F13" t="s">
-        <v>119</v>
-      </c>
-      <c r="G13" t="s">
-        <v>120</v>
-      </c>
-      <c r="H13" t="s">
-        <v>121</v>
       </c>
       <c r="I13" t="s">
         <v>60</v>
@@ -8896,15 +9133,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C5CD233-5B72-4F42-B23C-604FACAD3EAB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C5CD233-5B72-4F42-B23C-604FACAD3EAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3e4bc015-1695-4817-b784-4fdef86ad401"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C3BA748-FD44-422F-85CB-32E4B617A2AB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C3BA748-FD44-422F-85CB-32E4B617A2AB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46A052A9-20DB-493D-8BBE-1428CD8B950F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46A052A9-20DB-493D-8BBE-1428CD8B950F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3e4bc015-1695-4817-b784-4fdef86ad401"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>